<commit_message>
docs(init): ajuste na matriz SWOT, 5W2H e documentos de requisitos
</commit_message>
<xml_diff>
--- a/docs/matriz5w2h.xlsx
+++ b/docs/matriz5w2h.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alban\OneDrive\Área de Trabalho\Materias_FATEC\5_Semestre\lab_engenharia_de_software\documentação tg\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\albano\Desktop\Fatec\sexto_semestre\tg_licita_sp\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88FCF6C3-ADB5-4257-BD22-E554F78B62E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7136D40D-0ED2-49D1-BA96-830D0595C51F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,9 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -84,9 +87,6 @@
     <t>Backend e banco de dados</t>
   </si>
   <si>
-    <t>Ao planejar o sistema</t>
-  </si>
-  <si>
     <t>Fazer arquitetura modular e flexível</t>
   </si>
   <si>
@@ -141,9 +141,6 @@
     <t>Atingir usuários mobile e offline</t>
   </si>
   <si>
-    <t>Android/iOS</t>
-  </si>
-  <si>
     <t>Depois do lançamento web</t>
   </si>
   <si>
@@ -172,6 +169,12 @@
   </si>
   <si>
     <t>marketing</t>
+  </si>
+  <si>
+    <t>Ao planejar o sistema (fazer métodos reutilizavéis)</t>
+  </si>
+  <si>
+    <t>Android</t>
   </si>
 </sst>
 </file>
@@ -521,23 +524,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="90.26953125" customWidth="1"/>
-    <col min="2" max="2" width="53.7265625" customWidth="1"/>
-    <col min="3" max="3" width="60.1796875" customWidth="1"/>
-    <col min="4" max="4" width="35.81640625" customWidth="1"/>
+    <col min="1" max="1" width="90.21875" customWidth="1"/>
+    <col min="2" max="2" width="53.77734375" customWidth="1"/>
+    <col min="3" max="3" width="60.21875" customWidth="1"/>
+    <col min="4" max="4" width="35.77734375" customWidth="1"/>
     <col min="5" max="5" width="43" customWidth="1"/>
-    <col min="6" max="6" width="42.36328125" customWidth="1"/>
-    <col min="7" max="7" width="62.7265625" customWidth="1"/>
-    <col min="8" max="8" width="52.6328125" customWidth="1"/>
+    <col min="6" max="6" width="42.33203125" customWidth="1"/>
+    <col min="7" max="7" width="62.77734375" customWidth="1"/>
+    <col min="8" max="8" width="52.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -563,7 +566,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -589,7 +592,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -606,117 +609,117 @@
         <v>18</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="1" t="s">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="1" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="1" t="s">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="1" t="s">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>